<commit_message>
Added services dropdown and site footer
</commit_message>
<xml_diff>
--- a/Luxe_PriceList_Protected.xlsx
+++ b/Luxe_PriceList_Protected.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\luxehairartistryco-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCF12C8-C842-4CB6-A8A5-D01F4AF1E4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B92D156-5E5A-4D5F-BECB-66AC3F063357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9d9KDpfU8LGou9MeLU4ab9MXcnEzI/ZBqKrHC4Od8/+GEnqxvMfv/nCgygzXYwxqecBh3OggT+4z2/kWWvoTDQ==" workbookSaltValue="OJdOpa/zWVPuCGQluqTFuw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rhonda" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>Type</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>$150+</t>
-  </si>
-  <si>
-    <t>Scalp Massage</t>
   </si>
   <si>
     <t>END OF FORMULA</t>
@@ -878,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A937535C-4021-48F5-BE4F-0428B4806D4E}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1140,11 +1137,11 @@
         <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E18" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "group", name: "Scalp Massage", },</v>
+        <v>{type: "group", name: "Balayage", },</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,14 +1149,14 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="4">
-        <v>55</v>
+        <v>92</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="E19" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Scalp Massage", price: "$55", },</v>
+        <v>{type: "item", name: "Balayage", price: "$150+", },</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1167,11 +1164,11 @@
         <v>11</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E20" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "group", name: "Balayage", },</v>
+        <v>{type: "group", name: "Extensions", },</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,41 +1176,26 @@
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Balayage", price: "$150+", },</v>
+        <v>{type: "item", name: "Extensions", price: "$250+", },</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="E22" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "group", name: "Extensions", },</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="E23" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Extensions", price: "$250+", },</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2889,7 +2871,7 @@
     <row r="301" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="10"/>
       <c r="B301" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C301" s="12"/>
       <c r="D301" s="11"/>
@@ -2931,7 +2913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8144DD-65FC-4D8E-8EC4-E08A7884CF51}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
@@ -5233,7 +5215,7 @@
     <row r="301" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="10"/>
       <c r="B301" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C301" s="12"/>
       <c r="D301" s="11"/>

</xml_diff>

<commit_message>
Updated ArtistCardGroup to have external service list, added icon, updated bio & prices
</commit_message>
<xml_diff>
--- a/Luxe_PriceList_Protected.xlsx
+++ b/Luxe_PriceList_Protected.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\luxehairartistryco-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B92D156-5E5A-4D5F-BECB-66AC3F063357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA23F5C-F0E8-41BA-AED6-68C3E5C870A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9d9KDpfU8LGou9MeLU4ab9MXcnEzI/ZBqKrHC4Od8/+GEnqxvMfv/nCgygzXYwxqecBh3OggT+4z2/kWWvoTDQ==" workbookSaltValue="OJdOpa/zWVPuCGQluqTFuw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rhonda" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>Type</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>END OF FORMULA</t>
+  </si>
+  <si>
+    <t>$25+</t>
+  </si>
+  <si>
+    <t>$45+</t>
   </si>
 </sst>
 </file>
@@ -875,9 +881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A937535C-4021-48F5-BE4F-0428B4806D4E}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,12 +1088,12 @@
       <c r="B14" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="4">
-        <v>25</v>
+      <c r="C14" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="E14" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Wash &amp; Set", price: "$25", },</v>
+        <v>{type: "item", name: "Wash &amp; Set", price: "$25+", },</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1097,12 +1103,12 @@
       <c r="B15" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="4">
-        <v>45</v>
+      <c r="C15" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="E15" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Wash, Cut &amp; Style", price: "$45", },</v>
+        <v>{type: "item", name: "Wash, Cut &amp; Style", price: "$45+", },</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2913,7 +2919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8144DD-65FC-4D8E-8EC4-E08A7884CF51}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated Rhonda and Kim bio
</commit_message>
<xml_diff>
--- a/Luxe_PriceList_Protected.xlsx
+++ b/Luxe_PriceList_Protected.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\luxehairartistryco-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA23F5C-F0E8-41BA-AED6-68C3E5C870A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96059AE5-F8E8-4161-B012-EAA4C561A40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9d9KDpfU8LGou9MeLU4ab9MXcnEzI/ZBqKrHC4Od8/+GEnqxvMfv/nCgygzXYwxqecBh3OggT+4z2/kWWvoTDQ==" workbookSaltValue="OJdOpa/zWVPuCGQluqTFuw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rhonda" sheetId="3" r:id="rId1"/>
@@ -881,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A937535C-4021-48F5-BE4F-0428B4806D4E}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -2919,9 +2919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8144DD-65FC-4D8E-8EC4-E08A7884CF51}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3183,14 +3183,14 @@
         <v>63</v>
       </c>
       <c r="C16" s="4">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Express Pedi", price: "$40", description: "Foot soak, Nail trimmed and shaped finished with a hydrating cream.", },</v>
+        <v>{type: "item", name: "Express Pedi", price: "$45", description: "Foot soak, Nail trimmed and shaped finished with a hydrating cream.", },</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1.0.1: Updated Rhonda pricelist, added SVGs to asset folder
</commit_message>
<xml_diff>
--- a/Luxe_PriceList_Protected.xlsx
+++ b/Luxe_PriceList_Protected.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\luxehairartistryco-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96059AE5-F8E8-4161-B012-EAA4C561A40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7DD508-5FC0-4A99-B152-33601AB0A5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9d9KDpfU8LGou9MeLU4ab9MXcnEzI/ZBqKrHC4Od8/+GEnqxvMfv/nCgygzXYwxqecBh3OggT+4z2/kWWvoTDQ==" workbookSaltValue="OJdOpa/zWVPuCGQluqTFuw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rhonda" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
   <si>
     <t>Type</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>$45+</t>
+  </si>
+  <si>
+    <t>$115 to $175+</t>
+  </si>
+  <si>
+    <t>$85 to $105</t>
+  </si>
+  <si>
+    <t>$55 to $75</t>
   </si>
 </sst>
 </file>
@@ -881,9 +890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A937535C-4021-48F5-BE4F-0428B4806D4E}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,12 +1025,12 @@
       <c r="B9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="4">
-        <v>55</v>
+      <c r="C9" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="E9" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Partial Highlights", price: "$55", },</v>
+        <v>{type: "item", name: "Partial Highlights", price: "$55 to $75", },</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1031,12 +1040,12 @@
       <c r="B10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="4">
-        <v>75</v>
+      <c r="C10" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="E10" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "3/4 Head Highlights", price: "$75", },</v>
+        <v>{type: "item", name: "3/4 Head Highlights", price: "$85 to $105", },</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1046,12 +1055,12 @@
       <c r="B11" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="4">
-        <v>95</v>
+      <c r="C11" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="E11" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Full Highlights", price: "$95", },</v>
+        <v>{type: "item", name: "Full Highlights", price: "$115 to $175+", },</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2912,6 +2921,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2919,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8144DD-65FC-4D8E-8EC4-E08A7884CF51}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1.0.2: Updated Rhonda price list, Updated Victoria booking link
</commit_message>
<xml_diff>
--- a/Luxe_PriceList_Protected.xlsx
+++ b/Luxe_PriceList_Protected.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\luxehairartistryco-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Marttunen\Documents\luxehairartistryco-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7DD508-5FC0-4A99-B152-33601AB0A5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9d9KDpfU8LGou9MeLU4ab9MXcnEzI/ZBqKrHC4Od8/+GEnqxvMfv/nCgygzXYwxqecBh3OggT+4z2/kWWvoTDQ==" workbookSaltValue="OJdOpa/zWVPuCGQluqTFuw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDB9BA9-603F-4EF1-8369-FD292C1C8D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6EC0059-46D8-497B-99E1-DFA4A7A4168A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rhonda" sheetId="3" r:id="rId1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t>Type</t>
   </si>
@@ -327,15 +326,9 @@
     <t>$250+</t>
   </si>
   <si>
-    <t>$150+</t>
-  </si>
-  <si>
     <t>END OF FORMULA</t>
   </si>
   <si>
-    <t>$25+</t>
-  </si>
-  <si>
     <t>$45+</t>
   </si>
   <si>
@@ -346,6 +339,18 @@
   </si>
   <si>
     <t>$55 to $75</t>
+  </si>
+  <si>
+    <t>$175+</t>
+  </si>
+  <si>
+    <t>$50+</t>
+  </si>
+  <si>
+    <t>$28+</t>
+  </si>
+  <si>
+    <t>Cut &amp; Style</t>
   </si>
 </sst>
 </file>
@@ -890,22 +895,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A937535C-4021-48F5-BE4F-0428B4806D4E}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="100.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="100.7109375" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="12.7109375" style="1" hidden="1"/>
+    <col min="1" max="1" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="100.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="100.6640625" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -922,7 +927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -934,7 +939,7 @@
         <v>{type: "group", name: "Haircuts", },</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -942,14 +947,14 @@
         <v>77</v>
       </c>
       <c r="C3" s="4">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E3" s="15" t="str">
         <f t="shared" ref="E3:E66" si="0">IF(NOT($A3=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A3&amp;""", ", LOWER($B$1), ": """&amp;$B3&amp;""", ", IF(NOT($C3=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C3)=1, "$", ""), $C3, """, "), ""),  IF(NOT($D3=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D3&amp;""", "), ""), "},"), "")</f>
-        <v>{type: "item", name: "Woman's Haircut", price: "$30", },</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{type: "item", name: "Woman's Haircut", price: "$35", },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -957,14 +962,14 @@
         <v>78</v>
       </c>
       <c r="C4" s="4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E4" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Men's Haircut", price: "$22", },</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{type: "item", name: "Men's Haircut", price: "$25", },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -972,14 +977,14 @@
         <v>79</v>
       </c>
       <c r="C5" s="4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Kid's Haircut", price: "$22", },</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{type: "item", name: "Kid's Haircut", price: "$25", },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -991,7 +996,7 @@
         <v>{type: "group", name: "Colours", },</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1006,7 +1011,7 @@
         <v>{type: "item", name: "Colour", price: "$85+", },</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>{type: "group", name: "Highlights", },</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1026,14 +1031,14 @@
         <v>83</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E9" s="15" t="str">
         <f t="shared" si="0"/>
         <v>{type: "item", name: "Partial Highlights", price: "$55 to $75", },</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1041,14 +1046,14 @@
         <v>84</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>{type: "item", name: "3/4 Head Highlights", price: "$85 to $105", },</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -1056,14 +1061,14 @@
         <v>85</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E11" s="15" t="str">
         <f t="shared" si="0"/>
         <v>{type: "item", name: "Full Highlights", price: "$115 to $175+", },</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1075,1826 +1080,1834 @@
         <v>{type: "group", name: "Combos", },</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="4">
-        <v>35</v>
+        <v>88</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="E13" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Wash &amp; Cut", price: "$35", },</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{type: "item", name: "Wash &amp; Set", price: "$28+", },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
+      </c>
+      <c r="C14" s="4">
+        <v>40</v>
       </c>
       <c r="E14" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Wash &amp; Set", price: "$25+", },</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{type: "item", name: "Wash &amp; Cut", price: "$40", },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{type: "item", name: "Cut &amp; Style", price: "$45+", },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>{type: "item", name: "Wash, Cut &amp; Style", price: "$45+", },</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="C16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{type: "item", name: "Wash, Cut &amp; Style", price: "$50+", },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>{type: "group", name: "Toner", },</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="4">
+      <c r="E17" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{type: "group", name: "Toner", },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="4">
         <v>50</v>
       </c>
-      <c r="E17" s="15" t="str">
+      <c r="E18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>{type: "item", name: "Toner", price: "$50", },</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>{type: "group", name: "Balayage", },</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="E19" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>{type: "item", name: "Balayage", price: "$150+", },</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{type: "group", name: "Balayage", },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{type: "item", name: "Balayage", price: "$175+", },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>{type: "group", name: "Extensions", },</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{type: "group", name: "Extensions", },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="15" t="str">
+      <c r="E22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>{type: "item", name: "Extensions", price: "$250+", },</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C24" s="5"/>
       <c r="E24" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
       <c r="E25" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C26" s="5"/>
       <c r="E26" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
       <c r="E27" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E28" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C30" s="5"/>
       <c r="E30" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C31" s="5"/>
       <c r="E31" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C32" s="5"/>
       <c r="E32" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="6"/>
       <c r="E33" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E34" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E35" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E36" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E37" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E38" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E39" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E40" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E41" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E42" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E43" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E44" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E45" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E46" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E47" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E48" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="15" t="str">
         <f t="shared" ref="E67:E130" si="1">IF(NOT($A67=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A67&amp;""", ", LOWER($B$1), ": """&amp;$B67&amp;""", ", IF(NOT($C67=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C67)=1, "$", ""), $C67, """, "), ""),  IF(NOT($D67=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D67&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="15" t="str">
         <f t="shared" ref="E131:E194" si="2">IF(NOT($A131=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A131&amp;""", ", LOWER($B$1), ": """&amp;$B131&amp;""", ", IF(NOT($C131=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C131)=1, "$", ""), $C131, """, "), ""),  IF(NOT($D131=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D131&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="15" t="str">
         <f t="shared" ref="E195:E258" si="3">IF(NOT($A195=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A195&amp;""", ", LOWER($B$1), ": """&amp;$B195&amp;""", ", IF(NOT($C195=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C195)=1, "$", ""), $C195, """, "), ""),  IF(NOT($D195=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D195&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E220" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E221" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E222" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E223" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E224" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E225" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E226" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E227" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E228" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E229" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E230" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E231" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E232" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E233" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E234" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E235" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E236" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E237" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E238" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E239" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E240" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E241" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E242" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E243" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E244" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E245" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E246" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E247" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E248" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E249" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E250" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E251" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E252" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E253" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E254" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E255" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E256" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E257" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E258" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E259" s="15" t="str">
         <f t="shared" ref="E259:E300" si="4">IF(NOT($A259=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A259&amp;""", ", LOWER($B$1), ": """&amp;$B259&amp;""", ", IF(NOT($C259=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C259)=1, "$", ""), $C259, """, "), ""),  IF(NOT($D259=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D259&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E260" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E261" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E262" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E263" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E264" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E265" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E266" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E267" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E268" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E269" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E270" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E271" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E272" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E273" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E274" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E275" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E276" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E277" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E278" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E279" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E280" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E281" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E282" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E283" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E284" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E285" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E286" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E287" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E288" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E289" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E290" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E291" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E292" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E293" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E294" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E295" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E296" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E297" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E298" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E299" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E300" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A301" s="10"/>
       <c r="B301" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C301" s="12"/>
       <c r="D301" s="11"/>
       <c r="E301" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="O3sl82i5KK8ePPnB0+MCkZw+tA4/3TJwuGgffLHL3/U8uxEfAaCnyYG7XuEpX5qJSakdxwQW3xWStTxfouvsrA==" saltValue="P+vwxRyDqMpZHjThKKYlfA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="A2:D1048576">
+  <conditionalFormatting sqref="A2:D14 A23:D1048576 D15:D22 A16:C22">
     <cfRule type="expression" dxfId="9" priority="5">
       <formula>$A2="group"</formula>
     </cfRule>
@@ -2902,12 +2915,12 @@
       <formula>$A2="subgroup"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
+  <conditionalFormatting sqref="B2:B14 B16:B1048576">
     <cfRule type="expression" dxfId="7" priority="4">
       <formula>AND(NOT($A2=""), $B2="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="C2:C14 C16:C1048576">
     <cfRule type="expression" dxfId="6" priority="2">
       <formula>AND(OR($A2="group",$A2="subgroup"), NOT($C2=""))</formula>
     </cfRule>
@@ -2915,13 +2928,13 @@
       <formula>AND($A2="item", $C2="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{8FB5B616-9ABD-4D10-A0A7-971E8CB01D2D}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A14 A16:A1048576" xr:uid="{8FB5B616-9ABD-4D10-A0A7-971E8CB01D2D}">
       <formula1>"item, group, subgroup"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2934,17 +2947,17 @@
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="100.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="100.7109375" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="12.7109375" style="1" hidden="1"/>
+    <col min="1" max="1" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="100.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="100.6640625" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2961,7 +2974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -2973,7 +2986,7 @@
         <v>{type: "group", name: "Natural Nail Enhancements", },</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -2988,7 +3001,7 @@
         <v>{type: "subgroup", name: "BioSculpture Gel", description: "BioSculpture Gel is a Superior product making nails beautiful, flexible and durable, without any Damage. It is a one step system that strengthens and promotes the growth of natural nails. It is applied onto the natural nail or used to create strong and comfortable tips for added length. ", },</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -3006,7 +3019,7 @@
         <v>{type: "item", name: "Full Cover Tips", price: "$95", description: "Instantly creating perfect shape and length natural looking nails. BioSculptures Full Cover tips use soft gel adhesion technology to bring you the strongest most comfortable tips on the market. No Glue, odours, dust, fumes or excessive filing to preserve the health of your natural nail. ", },</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -3024,7 +3037,7 @@
         <v>{type: "item", name: "Overlay", price: "$65", description: "BioSculpture Gel is applied to the natural nail, it strengthens and promotes natural nail growth.  The Gel is cured under a UV light, leaving the nail strong but flexible with a natural glossy or high shine finish.", },</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -3042,7 +3055,7 @@
         <v>{type: "item", name: "Fill or Soak Off with Reapplication", price: "$70", description: "Reapplication of BioSculpture overlay. Depending on your nail type the gel will be rebalanced or removed with gel remover before a new application of nourishing gel. ", },</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>{type: "subgroup", name: "Evo by BioSculpture", description: "Evo is a revolutionary colour system that has evolved from the BioSculpture gel system. It boasts the latest technology in gel Formulations. Infused with Vitamin A and E leaving the naIl nourished and rehydrated  Evos medical grade formula maintains and promotes healthy natural nails. ", },</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
@@ -3075,7 +3088,7 @@
         <v>{type: "item", name: "Evo Gel Polish Manicure", price: "$65", description: "The Gel polish system consists of three base gels, each having a unique texture and purpose to treat different nail types. Applied to the Natural nail it is extremely durable, long lasting, high shine gel.", },</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>1</v>
       </c>
@@ -3093,7 +3106,7 @@
         <v>{type: "item", name: "Evo Gel Polish Pedicure  ", price: "$75", description: "Upgrade your signature pedicure for a long lasting, durable gel polish on your toes.  Service includes foot soak, nails trimmed and shaped, cuticle and callus work. Gel is applied to the nails. Complete the pedicure with a relaxing massage and exfoliation with sugar scrub then wrapped in a hot towel. ", },</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -3105,7 +3118,7 @@
         <v>{type: "subgroup", name: "Add-Ons", },</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -3120,7 +3133,7 @@
         <v>{type: "item", name: "Add Full Cover Tip", price: "$5 per Nail", },</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -3137,7 +3150,7 @@
 $30 per 10 Nails", },</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -3149,7 +3162,7 @@
         <v>{type: "group", name: "Fingers &amp; Toes", },</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>1</v>
       </c>
@@ -3167,7 +3180,7 @@
         <v>{type: "item", name: "Express Mani", price: "$30", description: "Nails trimmed and shaped,finished with a hydrating cream.", },</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>1</v>
       </c>
@@ -3185,7 +3198,7 @@
         <v>{type: "item", name: "Spa Manicure", price: "$50", description: "Nails shaped, cuticle work. Hands are massaged. Finish the treatment with a polish application.", },</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>1</v>
       </c>
@@ -3203,7 +3216,7 @@
         <v>{type: "item", name: "Express Pedi", price: "$45", description: "Foot soak, Nail trimmed and shaped finished with a hydrating cream.", },</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>1</v>
       </c>
@@ -3221,7 +3234,7 @@
         <v>{type: "item", name: "Sports Pedicure", price: "$55", description: "Foot soak, Nails trimmed and shaped, cuticle and callus work. Finished with a massage.", },</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
@@ -3239,7 +3252,7 @@
         <v>{type: "item", name: "Spa Pedicure", price: "$65 (Without Polish $60)", description: "Foot soak, Nails trimmed and shaped, cuticle and callus work. Feet are massaged and  exfoliated with sugar scrub wrapped in a hot towel. Finish the treatment with a polish application.", },</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>1</v>
       </c>
@@ -3257,7 +3270,7 @@
         <v>{type: "item", name: "Gentleman's Pedicure", price: "$60", description: "Foot soak, Nails trimmed and shaped, cuticle and callus work. Feet are massaged and  exfoliated with sugar scrub wrapped in a hot towel. ", },</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
@@ -3272,7 +3285,7 @@
         <v>{type: "group", name: "The B/S Brace System", description: "A NON-Surgical, corrective procedure that will eliminate pain and help correct the curvature of the nail", },</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>1</v>
       </c>
@@ -3287,7 +3300,7 @@
         <v>{type: "item", name: "Add Brace Nail", price: "$30", },</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>1</v>
       </c>
@@ -3302,7 +3315,7 @@
         <v>{type: "item", name: "Add 2 Brace Nails", price: "$50", },</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
@@ -3314,7 +3327,7 @@
         <v>{type: "group", name: "Lash Extensions", },</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>1</v>
       </c>
@@ -3329,7 +3342,7 @@
         <v>{type: "item", name: "Full Set", price: "$160", },</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>1</v>
       </c>
@@ -3344,7 +3357,7 @@
         <v>{type: "item", name: "2 Week Fill", price: "$60", },</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>1</v>
       </c>
@@ -3359,7 +3372,7 @@
         <v>{type: "item", name: "3 Week Fill", price: "$70", },</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>1</v>
       </c>
@@ -3374,7 +3387,7 @@
         <v>{type: "item", name: "4 Week Fill", price: "$80", },</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
@@ -3386,7 +3399,7 @@
         <v>{type: "group", name: "Waxing &amp; Sugaring", },</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>12</v>
       </c>
@@ -3398,7 +3411,7 @@
         <v>{type: "subgroup", name: "Face", },</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>1</v>
       </c>
@@ -3413,7 +3426,7 @@
         <v>{type: "item", name: "Brows", price: "$24", },</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>1</v>
       </c>
@@ -3428,7 +3441,7 @@
         <v>{type: "item", name: "Upper Lip", price: "$15", },</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>1</v>
       </c>
@@ -3443,7 +3456,7 @@
         <v>{type: "item", name: "Chin", price: "$18", },</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>1</v>
       </c>
@@ -3458,7 +3471,7 @@
         <v>{type: "item", name: "Full Face", price: "$45", },</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>12</v>
       </c>
@@ -3470,7 +3483,7 @@
         <v>{type: "subgroup", name: "Body", },</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>1</v>
       </c>
@@ -3485,7 +3498,7 @@
         <v>{type: "item", name: "Brazilian", price: "$70", },</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>1</v>
       </c>
@@ -3500,7 +3513,7 @@
         <v>{type: "item", name: "Bikini", price: "$45", },</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>1</v>
       </c>
@@ -3515,7 +3528,7 @@
         <v>{type: "item", name: "Extended Bikini", price: "$55", },</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>1</v>
       </c>
@@ -3530,7 +3543,7 @@
         <v>{type: "item", name: "Underarms", price: "$20", },</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>1</v>
       </c>
@@ -3545,7 +3558,7 @@
         <v>{type: "item", name: "Full Arm", price: "$30", },</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>1</v>
       </c>
@@ -3560,7 +3573,7 @@
         <v>{type: "item", name: "Full Leg", price: "$80", },</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>1</v>
       </c>
@@ -3575,7 +3588,7 @@
         <v>{type: "item", name: "Half Leg", price: "$45", },</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>12</v>
       </c>
@@ -3587,7 +3600,7 @@
         <v>{type: "subgroup", name: "Combo", },</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>1</v>
       </c>
@@ -3602,7 +3615,7 @@
         <v>{type: "item", name: "Brazilian + Full Leg", price: "$130", },</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>1</v>
       </c>
@@ -3617,7 +3630,7 @@
         <v>{type: "item", name: "Bikini + Full Leg", price: "$115", },</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>1</v>
       </c>
@@ -3632,7 +3645,7 @@
         <v>{type: "item", name: "Brazilian + Underarms", price: "$85", },</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>1</v>
       </c>
@@ -3647,7 +3660,7 @@
         <v>{type: "item", name: "Brows + Upper Lip", price: "$34", },</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>12</v>
       </c>
@@ -3659,7 +3672,7 @@
         <v>{type: "subgroup", name: "Men", },</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>1</v>
       </c>
@@ -3674,7 +3687,7 @@
         <v>{type: "item", name: "Chest", price: "$50", },</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>1</v>
       </c>
@@ -3689,7 +3702,7 @@
         <v>{type: "item", name: "Back", price: "$50", },</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>11</v>
       </c>
@@ -3701,7 +3714,7 @@
         <v>{type: "group", name: "Tinting", },</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>1</v>
       </c>
@@ -3716,7 +3729,7 @@
         <v>{type: "item", name: "Eyelashes", price: "$35", },</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>1</v>
       </c>
@@ -3731,7 +3744,7 @@
         <v>{type: "item", name: "Brows", price: "$25", },</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>1</v>
       </c>
@@ -3746,1492 +3759,1492 @@
         <v>{type: "item", name: "Brow Wax &amp; Tint", price: "$35", },</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E54" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E55" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E56" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E57" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E58" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E59" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E60" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E61" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E62" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E63" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E64" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="15" t="str">
         <f t="shared" ref="E67:E130" si="1">IF(NOT($A67=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A67&amp;""", ", LOWER($B$1), ": """&amp;$B67&amp;""", ", IF(NOT($C67=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C67)=1, "$", ""), $C67, """, "), ""),  IF(NOT($D67=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D67&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="15" t="str">
         <f t="shared" ref="E131:E194" si="2">IF(NOT($A131=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A131&amp;""", ", LOWER($B$1), ": """&amp;$B131&amp;""", ", IF(NOT($C131=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C131)=1, "$", ""), $C131, """, "), ""),  IF(NOT($D131=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D131&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="15" t="str">
         <f t="shared" ref="E195:E258" si="3">IF(NOT($A195=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A195&amp;""", ", LOWER($B$1), ": """&amp;$B195&amp;""", ", IF(NOT($C195=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C195)=1, "$", ""), $C195, """, "), ""),  IF(NOT($D195=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D195&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E220" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E221" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E222" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E223" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E224" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E225" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E226" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E227" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E228" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E229" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E230" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E231" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E232" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E233" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E234" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E235" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E236" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E237" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E238" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E239" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E240" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E241" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E242" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E243" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E244" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E245" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E246" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E247" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E248" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E249" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E250" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E251" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E252" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E253" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E254" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E255" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E256" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E257" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E258" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E259" s="15" t="str">
         <f t="shared" ref="E259:E300" si="4">IF(NOT($A259=""), _xlfn.CONCAT("{", LOWER($A$1), ": """&amp;$A259&amp;""", ", LOWER($B$1), ": """&amp;$B259&amp;""", ", IF(NOT($C259=""),_xlfn.CONCAT(LOWER($C$1), ": """, IF(TYPE($C259)=1, "$", ""), $C259, """, "), ""),  IF(NOT($D259=""),_xlfn.CONCAT(LOWER($D$1), ": """&amp;$D259&amp;""", "), ""), "},"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E260" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E261" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E262" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E263" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E264" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E265" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E266" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E267" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E268" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E269" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E270" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E271" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E272" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E273" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E274" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E275" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E276" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E277" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E278" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E279" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E280" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E281" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E282" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E283" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E284" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E285" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E286" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E287" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E288" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E289" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E290" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E291" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E292" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E293" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E294" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E295" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E296" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E297" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E298" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E299" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E300" s="15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A301" s="10"/>
       <c r="B301" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C301" s="12"/>
       <c r="D301" s="11"/>

</xml_diff>